<commit_message>
implement support for functions qlLeg(), qlMultiPhaseLeg(), qlSwap()
</commit_message>
<xml_diff>
--- a/Data2/XLS/EUR/EURSwap.xlsx
+++ b/Data2/XLS/EUR/EURSwap.xlsx
@@ -2183,7 +2183,7 @@
   <dimension ref="A1:T87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2199,10 +2199,9 @@
     <col min="10" max="11" width="16.5" style="24" customWidth="1" outlineLevel="1"/>
     <col min="12" max="12" width="20.1640625" style="24" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.83203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" style="24" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="7" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="9.33203125" style="2" collapsed="1"/>
-    <col min="17" max="16384" width="9.33203125" style="2"/>
+    <col min="14" max="14" width="17.83203125" style="24" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="7" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16384" width="9.33203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -2325,9 +2324,9 @@
       <c r="M3" s="141">
         <v>0</v>
       </c>
-      <c r="N3" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M3,L3,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="N3" s="1" t="str">
+        <f>_xll.qlLeg(EvaluationDate,,,,M3,L3)</f>
+        <v>obj_00867#0001</v>
       </c>
       <c r="O3" s="1" t="b">
         <v>1</v>
@@ -2376,16 +2375,16 @@
         <f>G27</f>
         <v>0</v>
       </c>
-      <c r="L4" s="142" t="e">
-        <f>_xll.qlCalendarAdvance($C$3,L3,"1D","f")</f>
-        <v>#NUM!</v>
+      <c r="L4" s="142">
+        <f>_xll.qlCalendarAdvance(,$C$3,L3,"1D","f")</f>
+        <v>42137</v>
       </c>
       <c r="M4" s="143">
         <v>0</v>
       </c>
-      <c r="N4" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M4,L4,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="N4" s="1" t="str">
+        <f>_xll.qlLeg(EvaluationDate,,,,M4,L4)</f>
+        <v>obj_0086b#0000</v>
       </c>
       <c r="O4" s="1" t="b">
         <f t="shared" ref="O4:O26" si="3">NOT(M4=0)</f>
@@ -2427,23 +2426,23 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J5" s="30" t="e">
-        <f ca="1">AdditionalCF</f>
-        <v>#NAME?</v>
+      <c r="J5" s="30" t="str">
+        <f>AdditionalCF</f>
+        <v>obj_00868#0000</v>
       </c>
       <c r="K5" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="L5" s="142" t="e">
-        <f>_xll.qlCalendarAdvance($C$3,L4,"1D","f")</f>
-        <v>#VALUE!</v>
+      <c r="L5" s="142">
+        <f>_xll.qlCalendarAdvance(,$C$3,L4,"1D","f")</f>
+        <v>42138</v>
       </c>
       <c r="M5" s="143">
         <v>0</v>
       </c>
-      <c r="N5" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M5,L5,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="N5" s="1" t="str">
+        <f>_xll.qlLeg(EvaluationDate,,,,M5,L5)</f>
+        <v>obj_00869#0000</v>
       </c>
       <c r="O5" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2487,16 +2486,16 @@
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="142" t="e">
-        <f>_xll.qlCalendarAdvance($C$3,L5,"1D","f")</f>
-        <v>#VALUE!</v>
+      <c r="L6" s="142">
+        <f>_xll.qlCalendarAdvance(,$C$3,L5,"1D","f")</f>
+        <v>42139</v>
       </c>
       <c r="M6" s="143">
         <v>0</v>
       </c>
-      <c r="N6" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M6,L6,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="N6" s="1" t="str">
+        <f>_xll.qlLeg(EvaluationDate,,,,M6,L6)</f>
+        <v>obj_0086a#0000</v>
       </c>
       <c r="O6" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2545,8 +2544,8 @@
         <v>0</v>
       </c>
       <c r="N7" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M7,L7,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M7,L7)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O7" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2595,8 +2594,8 @@
         <v>0</v>
       </c>
       <c r="N8" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M8,L8,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M8,L8)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O8" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2644,8 +2643,8 @@
         <v>0</v>
       </c>
       <c r="N9" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M9,L9,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M9,L9)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O9" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2694,8 +2693,8 @@
         <v>0</v>
       </c>
       <c r="N10" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M10,L10,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M10,L10)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O10" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2744,8 +2743,8 @@
         <v>0</v>
       </c>
       <c r="N11" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M11,L11,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M11,L11)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O11" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2792,8 +2791,8 @@
         <v>0</v>
       </c>
       <c r="N12" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M12,L12,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M12,L12)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O12" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2840,8 +2839,8 @@
         <v>0</v>
       </c>
       <c r="N13" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M13,L13,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M13,L13)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O13" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2884,8 +2883,8 @@
         <v>0</v>
       </c>
       <c r="N14" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M14,L14,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M14,L14)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O14" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2914,8 +2913,8 @@
         <v>0</v>
       </c>
       <c r="N15" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M15,L15,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M15,L15)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O15" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2962,8 +2961,8 @@
         <v>0</v>
       </c>
       <c r="N16" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M16,L16,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M16,L16)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O16" s="1" t="b">
         <f t="shared" si="3"/>
@@ -3010,8 +3009,8 @@
         <v>0</v>
       </c>
       <c r="N17" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M17,L17,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M17,L17)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O17" s="1" t="b">
         <f t="shared" si="3"/>
@@ -3058,8 +3057,8 @@
         <v>0</v>
       </c>
       <c r="N18" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M18,L18,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M18,L18)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O18" s="1" t="b">
         <f t="shared" si="3"/>
@@ -3108,8 +3107,8 @@
         <v>0</v>
       </c>
       <c r="N19" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M19,L19,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M19,L19)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O19" s="1" t="b">
         <f t="shared" si="3"/>
@@ -3156,8 +3155,8 @@
         <v>0</v>
       </c>
       <c r="N20" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M20,L20,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M20,L20)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O20" s="1" t="b">
         <f t="shared" si="3"/>
@@ -3206,8 +3205,8 @@
         <v>0</v>
       </c>
       <c r="N21" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M21,L21,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M21,L21)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O21" s="1" t="b">
         <f t="shared" si="3"/>
@@ -3256,8 +3255,8 @@
         <v>0</v>
       </c>
       <c r="N22" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M22,L22,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M22,L22)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O22" s="1" t="b">
         <f t="shared" si="3"/>
@@ -3308,8 +3307,8 @@
         <v>0</v>
       </c>
       <c r="N23" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M23,L23,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M23,L23)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O23" s="1" t="b">
         <f t="shared" si="3"/>
@@ -3362,8 +3361,8 @@
         <v>0</v>
       </c>
       <c r="N24" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M24,L24,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M24,L24)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O24" s="1" t="b">
         <f t="shared" si="3"/>
@@ -3410,8 +3409,8 @@
         <v>0</v>
       </c>
       <c r="N25" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M25,L25,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M25,L25)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O25" s="1" t="b">
         <f t="shared" si="3"/>
@@ -3460,8 +3459,8 @@
         <v>0</v>
       </c>
       <c r="N26" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M26,L26,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlLeg(EvaluationDate,,,,M26,L26)</f>
+        <v>#NUM!</v>
       </c>
       <c r="O26" s="1" t="b">
         <f t="shared" si="3"/>
@@ -3503,16 +3502,16 @@
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="142" t="e">
-        <f>_xll.qlCalendarAdjust($C$3,E8,$C$11)</f>
-        <v>#NUM!</v>
+      <c r="L27" s="142">
+        <f>_xll.qlCalendarAdjust(,$C$3,E8,$C$11)</f>
+        <v>45791</v>
       </c>
       <c r="M27" s="143">
         <v>0</v>
       </c>
-      <c r="N27" s="1" t="e">
-        <f ca="1">_xll.qlLeg(,M27,L27,,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="N27" s="1" t="str">
+        <f>_xll.qlLeg(EvaluationDate,,,,M27,L27)</f>
+        <v>obj_0086c#0000</v>
       </c>
       <c r="O27" s="1" t="b">
         <v>1</v>
@@ -3550,13 +3549,13 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="144"/>
-      <c r="M28" s="65" t="e">
-        <f ca="1">IF(ISBLANK(L28),N28,L28)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N28" s="26" t="e">
-        <f ca="1">_xll.qlMultiPhaseLeg(,_xll.ohFilter(N3:N27,O3:O27),FALSE)</f>
-        <v>#NAME?</v>
+      <c r="M28" s="65" t="str">
+        <f>IF(ISBLANK(L28),N28,L28)</f>
+        <v>obj_00868#0000</v>
+      </c>
+      <c r="N28" s="26" t="str">
+        <f>_xll.qlMultiPhaseLeg(,,,,N3:N6,FALSE)</f>
+        <v>obj_00868#0000</v>
       </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -3570,9 +3569,9 @@
         <v>41</v>
       </c>
       <c r="B29" s="132"/>
-      <c r="C29" s="19" t="e">
-        <f ca="1">_xll.qlSwap(B29,$J$3:$J$5,$K$3:$K$5)</f>
-        <v>#NAME?</v>
+      <c r="C29" s="19" t="str">
+        <f>_xll.qlSwap(,B29,,,$J$3:$J$5,$K$3:$K$5)</f>
+        <v>obj_0086d#0000</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="9"/>
@@ -3871,7 +3870,7 @@
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
     </row>
-    <row r="39" spans="1:20" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="71" t="s">
         <v>49</v>
       </c>
@@ -3900,7 +3899,7 @@
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
     </row>
-    <row r="40" spans="1:20" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A40" s="67" t="s">
         <v>50</v>
       </c>
@@ -3930,7 +3929,7 @@
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
     </row>
-    <row r="41" spans="1:20" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A41" s="67" t="s">
         <v>51</v>
       </c>
@@ -3960,7 +3959,7 @@
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
     </row>
-    <row r="42" spans="1:20" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A42" s="69" t="s">
         <v>42</v>
       </c>
@@ -3990,7 +3989,7 @@
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
     </row>
-    <row r="43" spans="1:20" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A43" s="150" t="s">
         <v>29</v>
       </c>
@@ -4017,7 +4016,7 @@
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
     </row>
-    <row r="44" spans="1:20" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
       <c r="B44" s="10"/>
       <c r="C44" s="9"/>
@@ -4039,7 +4038,7 @@
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
     </row>
-    <row r="45" spans="1:20" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="64" t="s">
         <v>20</v>
       </c>
@@ -4095,7 +4094,7 @@
       <c r="B47" s="85"/>
       <c r="C47" s="86" t="e">
         <f ca="1">_xll.qlInstrumentNPV(C45,SwapID)</f>
-        <v>#VALUE!</v>
+        <v>#NUM!</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -4144,14 +4143,14 @@
       <c r="B49" s="152"/>
       <c r="C49" s="153" t="e">
         <f ca="1">C$25-NPV/C$51/10000</f>
-        <v>#VALUE!</v>
+        <v>#NUM!</v>
       </c>
       <c r="D49" s="156"/>
       <c r="E49" s="156"/>
       <c r="F49" s="152"/>
       <c r="G49" s="153" t="e">
         <f ca="1">G$25-NPV/G$51/10000</f>
-        <v>#VALUE!</v>
+        <v>#NUM!</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>

</xml_diff>